<commit_message>
Working with Range and Active Cells
</commit_message>
<xml_diff>
--- a/Spreadsheets/SectionFiles/S4_ReferencingRanges_Start.xlsx
+++ b/Spreadsheets/SectionFiles/S4_ReferencingRanges_Start.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LG\Dropbox\VBAFiles\SectionFiles\Completed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balic\Documents\Programming\Excel-VBA-Excel-Macros\Spreadsheets\SectionFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9A7B6D-61F9-4C2E-A580-687DD815FC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9165" tabRatio="682"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="682" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Purpose" sheetId="8" r:id="rId1"/>
@@ -21,22 +22,36 @@
     <sheet name="Workbook" sheetId="9" r:id="rId7"/>
     <sheet name="Activity" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <definedNames>
+    <definedName name="LastOne">'Referencing Cells'!$A$10</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Leila Gharani</author>
   </authors>
   <commentList>
-    <comment ref="A8" authorId="0" shapeId="0">
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -65,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="101">
   <si>
     <t>Company</t>
   </si>
@@ -382,14 +397,17 @@
   <si>
     <t>Answer is in the project video and included in the complete version of this workbook in Module "ProjectActivity"</t>
   </si>
+  <si>
+    <t>Moved 2 down, 3 right</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -561,31 +579,29 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
@@ -602,10 +618,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -659,7 +673,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Comma 2" xfId="1"/>
+    <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
@@ -1214,9 +1228,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1254,7 +1268,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1360,7 +1374,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1502,354 +1516,349 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF006666"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" zeroHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.73046875" customWidth="1"/>
-    <col min="2" max="2" width="1.86328125" customWidth="1"/>
-    <col min="3" max="3" width="16.3984375" customWidth="1"/>
-    <col min="4" max="4" width="25.265625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="1.77734375" customWidth="1"/>
+    <col min="2" max="2" width="1.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="25.21875" style="19" customWidth="1"/>
     <col min="5" max="5" width="1" customWidth="1"/>
-    <col min="6" max="6" width="51.73046875" customWidth="1"/>
+    <col min="6" max="6" width="51.77734375" customWidth="1"/>
     <col min="7" max="7" width="2" customWidth="1"/>
-    <col min="8" max="8" width="30.86328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.59765625" customWidth="1"/>
-    <col min="10" max="10" width="2.73046875" customWidth="1"/>
-    <col min="11" max="11" width="6.86328125" customWidth="1"/>
+    <col min="8" max="8" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.5546875" customWidth="1"/>
+    <col min="10" max="10" width="2.77734375" customWidth="1"/>
+    <col min="11" max="11" width="6.88671875" customWidth="1"/>
     <col min="12" max="16384" width="9" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="38"/>
+      <c r="D1" s="34"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="19"/>
+      <c r="I1" s="17"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="38"/>
+      <c r="D2" s="34"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="19"/>
+      <c r="I2" s="17"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="38"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="19"/>
+      <c r="I3" s="17"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
-      <c r="B5" s="22"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="E5" s="22"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="2" t="s">
         <v>90</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" s="27" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="24"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
+    <row r="6" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="24"/>
-    </row>
-    <row r="7" spans="1:12" s="33" customFormat="1" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="28"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="30" t="s">
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" s="29" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="29"/>
-      <c r="F7" s="31" t="s">
+      <c r="E7" s="25"/>
+      <c r="F7" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="28"/>
-    </row>
-    <row r="8" spans="1:12" s="33" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A8" s="28"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="35" t="s">
+      <c r="L7" s="24"/>
+    </row>
+    <row r="8" spans="1:12" s="29" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="24"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="34"/>
-      <c r="F8" s="36" t="s">
+      <c r="E8" s="30"/>
+      <c r="F8" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="28"/>
-    </row>
-    <row r="9" spans="1:12" s="33" customFormat="1" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A9" s="28"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="35" t="s">
+      <c r="L8" s="24"/>
+    </row>
+    <row r="9" spans="1:12" s="29" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="24"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="36" t="s">
+      <c r="E9" s="30"/>
+      <c r="F9" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="G9" s="36"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="28"/>
-    </row>
-    <row r="10" spans="1:12" s="33" customFormat="1" ht="57" x14ac:dyDescent="0.45">
-      <c r="A10" s="28"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="35" t="s">
+      <c r="L9" s="24"/>
+    </row>
+    <row r="10" spans="1:12" s="29" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="24"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="36" t="s">
+      <c r="E10" s="30"/>
+      <c r="F10" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="28"/>
-    </row>
-    <row r="11" spans="1:12" s="33" customFormat="1" ht="31.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="28"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="35" t="s">
+      <c r="L10" s="24"/>
+    </row>
+    <row r="11" spans="1:12" s="29" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="24"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="36" t="s">
+      <c r="E11" s="30"/>
+      <c r="F11" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="G11" s="36"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="28"/>
-    </row>
-    <row r="12" spans="1:12" s="33" customFormat="1" ht="31.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="28"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="35" t="s">
+      <c r="L11" s="24"/>
+    </row>
+    <row r="12" spans="1:12" s="29" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="24"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="E12" s="34"/>
-      <c r="F12" s="36" t="s">
+      <c r="E12" s="30"/>
+      <c r="F12" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="G12" s="36"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="28"/>
-    </row>
-    <row r="13" spans="1:12" s="33" customFormat="1" ht="47.25" x14ac:dyDescent="0.45">
-      <c r="A13" s="28"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="35" t="s">
+      <c r="L12" s="24"/>
+    </row>
+    <row r="13" spans="1:12" s="29" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="24"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="E13" s="34"/>
-      <c r="F13" s="37" t="s">
+      <c r="E13" s="30"/>
+      <c r="F13" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="28"/>
-    </row>
-    <row r="14" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="28"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
+      <c r="L13" s="24"/>
+    </row>
+    <row r="14" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="24"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
       <c r="K14" s="1"/>
-      <c r="L14" s="28"/>
-    </row>
-    <row r="15" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="28"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
+      <c r="L14" s="24"/>
+    </row>
+    <row r="15" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="24"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="28"/>
-    </row>
-    <row r="16" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="28"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
+      <c r="L15" s="24"/>
+    </row>
+    <row r="16" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="24"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
       <c r="K16" s="1"/>
-      <c r="L16" s="28"/>
-    </row>
-    <row r="17" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
+      <c r="L16" s="24"/>
+    </row>
+    <row r="17" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="28"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-    </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.45"/>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.45"/>
+      <c r="L17" s="24"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C7" location="'Referencing Cells'!A1" display="Referencing Cells"/>
-    <hyperlink ref="C8" location="'Example_P_M'!A1" display="Example_P_M"/>
-    <hyperlink ref="C9" location="'Range_Reference'!A1" display="Range_Reference"/>
-    <hyperlink ref="C10" location="'Copy_Resize'!A1" display="Copy_Resize"/>
-    <hyperlink ref="C11" location="Worksheet!A1" display="Worksheet"/>
-    <hyperlink ref="C13" location="'Activity'!A1" display="Activity"/>
-    <hyperlink ref="C12" location="Workbook!A1" display="Workbook"/>
+    <hyperlink ref="C7" location="'Referencing Cells'!A1" display="Referencing Cells" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C8" location="'Example_P_M'!A1" display="Example_P_M" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C9" location="'Range_Reference'!A1" display="Range_Reference" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C10" location="'Copy_Resize'!A1" display="Copy_Resize" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C11" location="Worksheet!A1" display="Worksheet" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C13" location="'Activity'!A1" display="Activity" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C12" location="Workbook!A1" display="Workbook" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="95" orientation="landscape" r:id="rId1"/>
@@ -1858,22 +1867,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2">
     <tabColor theme="2" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="D3:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.73046875" customWidth="1"/>
-    <col min="3" max="3" width="10.73046875" customWidth="1"/>
+    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" customWidth="1"/>
+    <col min="10" max="10" width="10.77734375" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="4:4" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1881,7 +1905,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3">
     <tabColor theme="2" tint="-0.499984740745262"/>
   </sheetPr>
@@ -1891,13 +1915,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.265625" customWidth="1"/>
+    <col min="1" max="1" width="19.21875" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>50</v>
       </c>
@@ -1907,10 +1931,10 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6" ht="10.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="3" spans="1:6" ht="10.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="1:6" ht="10.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:6" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:6" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1918,17 +1942,17 @@
         <v>10200</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="13"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="14"/>
+      <c r="B7" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1937,24 +1961,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4">
     <tabColor theme="2" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.265625" customWidth="1"/>
-    <col min="2" max="2" width="10.265625" customWidth="1"/>
-    <col min="7" max="8" width="4.46484375" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" customWidth="1"/>
+    <col min="7" max="8" width="4.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>59</v>
       </c>
@@ -1964,9 +1988,9 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1986,7 +2010,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2005,9 +2029,9 @@
       <c r="F5" s="5">
         <v>10404</v>
       </c>
-      <c r="J5" s="12"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="J5" s="10"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2026,12 +2050,12 @@
       <c r="F6" s="5">
         <v>12484.800000000001</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="13"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K6" s="11"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2050,12 +2074,12 @@
       <c r="F7" s="5">
         <v>14981.76</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K7" s="13"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K7" s="11"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2075,12 +2099,12 @@
       <c r="F8" s="5">
         <v>17978.111999999997</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="K8" s="13"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K8" s="11"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2099,12 +2123,12 @@
       <c r="F9" s="5">
         <v>10506</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="K9" s="13"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K9" s="11"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2123,12 +2147,12 @@
       <c r="F10" s="5">
         <v>12607.2</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="13"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K10" s="11"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2147,12 +2171,12 @@
       <c r="F11" s="5">
         <v>15128.64</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="K11" s="13"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K11" s="11"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -2171,12 +2195,12 @@
       <c r="F12" s="5">
         <v>18154.367999999999</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="J12" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="K12" s="13"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="K12" s="11"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -2196,7 +2220,7 @@
         <v>10608</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -2217,7 +2241,7 @@
         <v>12729.6</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -2237,7 +2261,7 @@
         <v>15275.52</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -2257,7 +2281,7 @@
         <v>20400</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -2277,7 +2301,7 @@
         <v>24480</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -2297,7 +2321,7 @@
         <v>29376</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -2317,7 +2341,7 @@
         <v>35251.199999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -2337,7 +2361,7 @@
         <v>42301.440000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -2357,7 +2381,7 @@
         <v>50761.728000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -2377,7 +2401,7 @@
         <v>10710</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -2398,7 +2422,7 @@
         <v>21573.734399999998</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -2418,7 +2442,7 @@
         <v>25888.48128</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -2438,7 +2462,7 @@
         <v>31066.177535999996</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -2458,7 +2482,7 @@
         <v>10404</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -2478,7 +2502,7 @@
         <v>12484.800000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -2498,7 +2522,7 @@
         <v>14981.76</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -2518,27 +2542,26 @@
         <v>10302</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="10" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" t="s">
         <v>43</v>
       </c>
       <c r="E30" s="9">
         <v>10300</v>
       </c>
-      <c r="F30" s="11">
+      <c r="F30" s="5">
         <v>10506</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2546,7 +2569,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5">
     <tabColor theme="2" tint="-0.499984740745262"/>
   </sheetPr>
@@ -2556,15 +2579,15 @@
       <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.86328125" customWidth="1"/>
-    <col min="7" max="7" width="2.265625" customWidth="1"/>
-    <col min="8" max="8" width="1.265625" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" customWidth="1"/>
+    <col min="7" max="7" width="2.21875" customWidth="1"/>
+    <col min="8" max="8" width="1.21875" customWidth="1"/>
     <col min="9" max="9" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>66</v>
       </c>
@@ -2574,8 +2597,8 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
         <v>61</v>
       </c>
       <c r="B2" s="8"/>
@@ -2583,18 +2606,18 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="15" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -2607,14 +2630,14 @@
       <c r="D4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2627,15 +2650,15 @@
       <c r="D5" s="5">
         <v>10404</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="14">
         <f>C5/D5-1</f>
         <v>-1.9607843137254943E-2</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2648,15 +2671,15 @@
       <c r="D6" s="5">
         <v>12484.800000000001</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="14">
         <f t="shared" ref="E6:E10" si="0">C6/D6-1</f>
         <v>-1.9607843137254943E-2</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2669,15 +2692,15 @@
       <c r="D7" s="5">
         <v>14981.76</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="14">
         <f t="shared" si="0"/>
         <v>-1.9607843137254943E-2</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2691,15 +2714,15 @@
       <c r="D8" s="5">
         <v>17978.111999999997</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="14">
         <f t="shared" si="0"/>
         <v>0.10000000000000009</v>
       </c>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2712,15 +2735,15 @@
       <c r="D9" s="5">
         <v>10506</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="14">
         <f t="shared" si="0"/>
         <v>-1.9607843137254943E-2</v>
       </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2733,121 +2756,110 @@
       <c r="D10" s="5">
         <v>12607.2</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="14">
         <f t="shared" si="0"/>
         <v>-1.9607843137254943E-2</v>
       </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A18" s="17" t="s">
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="17" t="s">
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="15" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2857,7 +2869,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6">
     <tabColor theme="2" tint="-0.499984740745262"/>
   </sheetPr>
@@ -2867,9 +2879,9 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>68</v>
       </c>
@@ -2886,7 +2898,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet7">
     <tabColor theme="2" tint="-0.499984740745262"/>
   </sheetPr>
@@ -2896,9 +2908,9 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>92</v>
       </c>
@@ -2908,17 +2920,17 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -2929,7 +2941,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet8">
     <tabColor theme="7" tint="0.79998168889431442"/>
   </sheetPr>
@@ -2937,9 +2949,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>91</v>
       </c>
@@ -2953,27 +2965,27 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>1</v>
       </c>
@@ -2981,7 +2993,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>2</v>
       </c>
@@ -2989,7 +3001,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>3</v>
       </c>
@@ -2997,7 +3009,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>4</v>
       </c>
@@ -3005,15 +3017,15 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B12" s="12" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="10" t="s">
         <v>77</v>
       </c>
       <c r="C12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>79</v>
       </c>
@@ -3021,8 +3033,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B16" s="20" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="18" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>